<commit_message>
final P06 + final scrum sheet
</commit_message>
<xml_diff>
--- a/P06/store/Scrum.xlsx
+++ b/P06/store/Scrum.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcia/Desktop/cse1325/P06/store/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{541FF94C-29CC-4541-A226-F95A169BDCF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D4082AC-6394-514D-9708-E569CD136D7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="178">
   <si>
     <t>Product Name:</t>
   </si>
@@ -545,16 +545,37 @@
     <t>Completed Day 5</t>
   </si>
   <si>
-    <t>Not Started</t>
-  </si>
-  <si>
-    <t>In Work</t>
-  </si>
-  <si>
     <t>Write the MainWin class, following the UML Diagram</t>
   </si>
   <si>
-    <t>Implement all its necessary methods</t>
+    <t>Write the onInsertCustomerClick method</t>
+  </si>
+  <si>
+    <t>Create a basic implementation of the ELSA Window GUI</t>
+  </si>
+  <si>
+    <t>Write the onInsertOptionClick method</t>
+  </si>
+  <si>
+    <t>Write the onInsertComputerClick method</t>
+  </si>
+  <si>
+    <t>Implement the OnViewClick method</t>
+  </si>
+  <si>
+    <t>basic implementation of the toolbar</t>
+  </si>
+  <si>
+    <t>add all the necessary images icons</t>
+  </si>
+  <si>
+    <t>Write the onAboutClick</t>
+  </si>
+  <si>
+    <t>Completed Day 7</t>
+  </si>
+  <si>
+    <t>Finished in Sprint 2</t>
   </si>
 </sst>
 </file>
@@ -1083,16 +1104,16 @@
                   <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>18</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>18</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>18</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1691,28 +1712,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3753,8 +3774,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+    <sheetView topLeftCell="A22" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3988,11 +4009,11 @@
       </c>
       <c r="B14" s="5">
         <f>B13-C14</f>
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C14" s="9">
         <f>COUNTIF(G$24:G$106,"Finished in Sprint 2")</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="5"/>
@@ -4012,7 +4033,7 @@
       </c>
       <c r="B15" s="5">
         <f>B14-C15</f>
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C15" s="9">
         <f>COUNTIF(G$24:G$106,"Finished in Sprint 3")</f>
@@ -4036,7 +4057,7 @@
       </c>
       <c r="B16" s="5">
         <f>B15-C16</f>
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C16" s="9">
         <f>COUNTIF(G$24:G$106,"Finished in Sprint 4")</f>
@@ -4056,7 +4077,7 @@
       </c>
       <c r="B17" s="5">
         <f>B16-C17</f>
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C17" s="9">
         <f>COUNTIF(G$24:G$106,"Finished in Sprint 4")</f>
@@ -4350,7 +4371,7 @@
         <v>2</v>
       </c>
       <c r="G29" s="17" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="H29" s="18" t="s">
         <v>31</v>
@@ -4383,7 +4404,7 @@
         <v>2</v>
       </c>
       <c r="G30" s="17" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="H30" s="18" t="s">
         <v>31</v>
@@ -4416,7 +4437,7 @@
         <v>2</v>
       </c>
       <c r="G31" s="17" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="H31" s="18" t="s">
         <v>31</v>
@@ -4447,7 +4468,7 @@
         <v>2</v>
       </c>
       <c r="G32" s="17" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="H32" s="18" t="s">
         <v>31</v>
@@ -4478,7 +4499,7 @@
         <v>2</v>
       </c>
       <c r="G33" s="17" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="H33" s="18" t="s">
         <v>31</v>
@@ -4511,7 +4532,7 @@
         <v>2</v>
       </c>
       <c r="G34" s="17" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="H34" s="18" t="s">
         <v>31</v>
@@ -4540,8 +4561,12 @@
       <c r="E35" s="42">
         <v>2</v>
       </c>
-      <c r="F35" s="17"/>
-      <c r="G35" s="17"/>
+      <c r="F35" s="17">
+        <v>2</v>
+      </c>
+      <c r="G35" s="17" t="s">
+        <v>177</v>
+      </c>
       <c r="H35" s="18" t="s">
         <v>70</v>
       </c>
@@ -5707,7 +5732,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView topLeftCell="A14" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
@@ -6945,8 +6970,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -7051,7 +7076,7 @@
       </c>
       <c r="B7" s="25">
         <f>COUNTA(D17:D995)</f>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C7" s="25"/>
       <c r="D7" s="25"/>
@@ -7066,7 +7091,7 @@
       </c>
       <c r="B8" s="25">
         <f t="shared" ref="B8:B14" si="0">B7-C8</f>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C8" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 1")</f>
@@ -7084,7 +7109,7 @@
       </c>
       <c r="B9" s="25">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C9" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 2")</f>
@@ -7102,7 +7127,7 @@
       </c>
       <c r="B10" s="25">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C10" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 3")</f>
@@ -7120,7 +7145,7 @@
       </c>
       <c r="B11" s="25">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C11" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 4")</f>
@@ -7138,7 +7163,7 @@
       </c>
       <c r="B12" s="25">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C12" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 5")</f>
@@ -7156,7 +7181,7 @@
       </c>
       <c r="B13" s="25">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C13" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 6")</f>
@@ -7174,11 +7199,11 @@
       </c>
       <c r="B14" s="25">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C14" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 7")</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D14" s="25"/>
       <c r="E14" s="25"/>
@@ -7225,10 +7250,10 @@
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="44" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E17" s="37" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="F17" s="38"/>
     </row>
@@ -7241,83 +7266,123 @@
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="39" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E18" s="37" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="F18" s="38"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A19" s="4">
         <v>3</v>
       </c>
       <c r="B19" s="35" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C19" s="4"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="37"/>
+      <c r="D19" s="39" t="s">
+        <v>168</v>
+      </c>
+      <c r="E19" s="37" t="s">
+        <v>176</v>
+      </c>
       <c r="F19" s="38"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A20" s="4">
         <v>4</v>
       </c>
-      <c r="B20" s="35"/>
+      <c r="B20" s="35" t="s">
+        <v>57</v>
+      </c>
       <c r="C20" s="4"/>
-      <c r="D20" s="39"/>
-      <c r="E20" s="37"/>
+      <c r="D20" s="39" t="s">
+        <v>170</v>
+      </c>
+      <c r="E20" s="37" t="s">
+        <v>176</v>
+      </c>
       <c r="F20" s="38"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A21" s="4">
         <v>5</v>
       </c>
-      <c r="B21" s="35"/>
+      <c r="B21" s="35" t="s">
+        <v>59</v>
+      </c>
       <c r="C21" s="4"/>
-      <c r="D21" s="39"/>
-      <c r="E21" s="37"/>
+      <c r="D21" s="39" t="s">
+        <v>171</v>
+      </c>
+      <c r="E21" s="37" t="s">
+        <v>176</v>
+      </c>
       <c r="F21" s="38"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A22" s="4">
         <v>6</v>
       </c>
-      <c r="B22" s="35"/>
+      <c r="B22" s="35" t="s">
+        <v>61</v>
+      </c>
       <c r="C22" s="4"/>
-      <c r="D22" s="39"/>
-      <c r="E22" s="37"/>
+      <c r="D22" s="39" t="s">
+        <v>172</v>
+      </c>
+      <c r="E22" s="37" t="s">
+        <v>176</v>
+      </c>
       <c r="F22" s="38"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A23" s="4">
         <v>7</v>
       </c>
-      <c r="B23" s="35"/>
+      <c r="B23" s="35" t="s">
+        <v>65</v>
+      </c>
       <c r="C23" s="4"/>
-      <c r="D23" s="39"/>
-      <c r="E23" s="37"/>
+      <c r="D23" s="39" t="s">
+        <v>173</v>
+      </c>
+      <c r="E23" s="37" t="s">
+        <v>176</v>
+      </c>
       <c r="F23" s="38"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A24" s="4">
         <v>8</v>
       </c>
-      <c r="B24" s="35"/>
+      <c r="B24" s="35" t="s">
+        <v>65</v>
+      </c>
       <c r="C24" s="4"/>
-      <c r="D24" s="39"/>
-      <c r="E24" s="37"/>
+      <c r="D24" s="39" t="s">
+        <v>174</v>
+      </c>
+      <c r="E24" s="37" t="s">
+        <v>176</v>
+      </c>
       <c r="F24" s="38"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A25" s="4">
         <v>9</v>
       </c>
-      <c r="B25" s="35"/>
+      <c r="B25" s="35" t="s">
+        <v>69</v>
+      </c>
       <c r="C25" s="4"/>
-      <c r="D25" s="39"/>
-      <c r="E25" s="37"/>
+      <c r="D25" s="39" t="s">
+        <v>175</v>
+      </c>
+      <c r="E25" s="37" t="s">
+        <v>176</v>
+      </c>
       <c r="F25" s="38"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.15">

</xml_diff>